<commit_message>
Better UI, new about window and rolling animation
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\RollCall\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\RandomCall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A9D1CC-B00B-4B7E-A3C6-F6E392840B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA818C0-CAB0-49D2-80B0-59C13005F48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="4476" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4212" yWindow="1428" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,25 +25,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>名字依次向下</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Dan_Evan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MeltIce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Astral</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>minqwq</t>
+    <t>麦克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>富兰克林</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>崔佛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莱斯特</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西米恩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>史崔奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉玛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吉米</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>戴夫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杰伊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>马丁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>德温</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汤雅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>强尼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小罗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈伟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈陶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奥尼尔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿曼达</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大厨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陶艾迪</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -399,7 +467,97 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>